<commit_message>
feat: activity to read, write and append from excel
</commit_message>
<xml_diff>
--- a/supportingData/simpleVariable.xlsx
+++ b/supportingData/simpleVariable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\MscIT\Sem 3\Pract\RPA\PracticalList\supportingData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\MscIT\Sem 3\Pract\RPA supporting docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4850A89C-5748-45CE-B355-AC6F707EBD9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB93EB1-7343-4810-AA67-8929E333462A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5205" yWindow="0" windowWidth="10500" windowHeight="8715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <t>Salary</t>
   </si>
   <si>
-    <t>Year</t>
+    <t>Years</t>
   </si>
 </sst>
 </file>
@@ -348,52 +348,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>20000</v>
+        <v>2019</v>
       </c>
       <c r="B2">
-        <v>2020</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>25000</v>
+        <v>2020</v>
       </c>
       <c r="B3">
-        <v>2021</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>2021</v>
+      </c>
+      <c r="B4">
         <v>35000</v>
-      </c>
-      <c r="B4">
-        <v>2022</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>2022</v>
+      </c>
+      <c r="B5">
         <v>40000</v>
       </c>
-      <c r="B5">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>2023</v>
+      </c>
+      <c r="B6">
+        <v>50000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>